<commit_message>
modifica grafica matrice di tracciabilità
</commit_message>
<xml_diff>
--- a/Documentazione/Testing_docs/Matrice di tracciabilità.xlsx
+++ b/Documentazione/Testing_docs/Matrice di tracciabilità.xlsx
@@ -396,8 +396,7 @@
     <t>L’utente meno esperto può interagire facilmente con il sistema poiché di comoda comprensione</t>
   </si>
   <si>
-    <t>DG_11
-Facilità d’uso</t>
+    <t>DG_11 Facilità d’uso</t>
   </si>
   <si>
     <t>RNF_U_2</t>
@@ -409,8 +408,7 @@
     <t>Facile</t>
   </si>
   <si>
-    <t>DG_12
-Interfaccia
+    <t>DG_12 Interfaccia
 intuitiva</t>
   </si>
   <si>
@@ -420,8 +418,7 @@
     <t>Ogni azione deve fornire un feedback chiaro, permettendo all'utente di comprendere e valutare facilmente il cambiamento.</t>
   </si>
   <si>
-    <t>DG_13
-Feedback
+    <t>DG_13 Feedback
 esplicito</t>
   </si>
   <si>
@@ -449,8 +446,7 @@
     <t>Il sistema deve garantire che tutte le operazioni avvengono con successo.</t>
   </si>
   <si>
-    <t>DG_4
-Affidabilità delle operazioni</t>
+    <t>DG_4 Affidabilità delle operazioni</t>
   </si>
   <si>
     <t>RNF_A_2</t>
@@ -459,8 +455,7 @@
     <t xml:space="preserve">Il sistema deve garantire un alto livello di sicurezza per preservare le informazioni sensibili. </t>
   </si>
   <si>
-    <t>DG_8
-Sicurezza dei dati</t>
+    <t>DG_8 Sicurezza dei dati</t>
   </si>
   <si>
     <t>RNF_A_3</t>
@@ -469,8 +464,7 @@
     <t>Il sistema deve sapersi comportare in situazioni di fallimento notificando l’utente, tramite appositi messaggi, l’errore e aiutarlo a completare le operazioni che stava svolgendo</t>
   </si>
   <si>
-    <t>DG_5
-Fallimento di
+    <t>DG_5 Fallimento di
 sistema</t>
   </si>
   <si>
@@ -486,8 +480,7 @@
     <t>Il sistema deve garantire la separazione netta delle operazioni sulla base degli utenti che possono effettuarle.</t>
   </si>
   <si>
-    <t>DG_6
-Gestione
+    <t>DG_6 Gestione
 permessi</t>
   </si>
   <si>
@@ -503,8 +496,7 @@
     <t>Il sistema dovrà essere correttamente funzionante anche con più di un utente connesso in contemporanea</t>
   </si>
   <si>
-    <t>DG_3
-Navigazione
+    <t>DG_3 Navigazione
 concorrente</t>
   </si>
   <si>
@@ -514,8 +506,7 @@
     <t>Il sistema dovrà garantire un’alta capacità di memorizzazione per poter conservare tutte le informazioni necessarie al suo funzionamento.</t>
   </si>
   <si>
-    <t>DG_2
-Quantità di dati</t>
+    <t>DG_2 Quantità di dati</t>
   </si>
   <si>
     <t>RNF_P_4</t>
@@ -524,8 +515,7 @@
     <t xml:space="preserve">Il sistema dovrà essere disponibile 24 ore su 24. </t>
   </si>
   <si>
-    <t>DG_7
-Disponibilità del
+    <t>DG_7 Disponibilità del
 sistema</t>
   </si>
   <si>
@@ -541,8 +531,7 @@
     <t>Il sistema deve essere sviluppato rispettando gli standard per garantire una buona manutenibilità.</t>
   </si>
   <si>
-    <t>DG_9
-Manutenibilità</t>
+    <t>DG_9 Manutenibilità</t>
   </si>
   <si>
     <t>RNF_S_2</t>
@@ -551,8 +540,7 @@
     <t>ll sistema deve essere sviluppato seguendo gli standard che assicurano una buona estensibilità delle funzionalità.</t>
   </si>
   <si>
-    <t>DG_10
-Estensibilità</t>
+    <t>DG_10 Estensibilità</t>
   </si>
   <si>
     <t>RNF_IM_1</t>
@@ -1921,7 +1909,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="25" t="s">
         <v>79</v>
       </c>
@@ -2077,7 +2065,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" ht="51.0" customHeight="1">
+    <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="25" t="s">
         <v>96</v>
       </c>
@@ -2337,7 +2325,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" ht="17.25" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>108</v>
       </c>
@@ -2573,7 +2561,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" ht="18.75" customHeight="1">
       <c r="A29" s="52" t="s">
         <v>122</v>
       </c>
@@ -2625,7 +2613,7 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" ht="19.5" customHeight="1">
       <c r="A30" s="25" t="s">
         <v>125</v>
       </c>
@@ -2677,7 +2665,7 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" ht="18.0" customHeight="1">
       <c r="A31" s="29" t="s">
         <v>129</v>
       </c>
@@ -2885,7 +2873,7 @@
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
     </row>
-    <row r="35">
+    <row r="35" ht="19.5" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>138</v>
       </c>
@@ -2937,7 +2925,7 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36">
+    <row r="36" ht="20.25" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>141</v>
       </c>
@@ -2989,7 +2977,7 @@
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
     </row>
-    <row r="37">
+    <row r="37" ht="19.5" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>144</v>
       </c>
@@ -3093,7 +3081,7 @@
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
     </row>
-    <row r="39">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>149</v>
       </c>
@@ -3197,7 +3185,7 @@
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
     </row>
-    <row r="41">
+    <row r="41" ht="18.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>154</v>
       </c>
@@ -3249,7 +3237,7 @@
       <c r="Y41" s="6"/>
       <c r="Z41" s="6"/>
     </row>
-    <row r="42">
+    <row r="42" ht="18.0" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>157</v>
       </c>
@@ -3301,7 +3289,7 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
     </row>
-    <row r="43">
+    <row r="43" ht="16.5" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>160</v>
       </c>
@@ -3405,7 +3393,7 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
     </row>
-    <row r="45">
+    <row r="45" ht="16.5" customHeight="1">
       <c r="A45" s="29" t="s">
         <v>165</v>
       </c>
@@ -3457,7 +3445,7 @@
       <c r="Y45" s="6"/>
       <c r="Z45" s="6"/>
     </row>
-    <row r="46" ht="32.25" customHeight="1">
+    <row r="46" ht="16.5" customHeight="1">
       <c r="A46" s="59" t="s">
         <v>168</v>
       </c>

</xml_diff>